<commit_message>
Update Validation data - LBM.xlsx
</commit_message>
<xml_diff>
--- a/data/Validation data - LBM.xlsx
+++ b/data/Validation data - LBM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20366"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lbrice1\Dropbox\LSU\PSE@LSU\PEMFC\Joule 2020\FCSDAT_Repository\FCSDAT\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisa\Dropbox\LSU\PSE@LSU\PEMFC\Joule_2020\FCSDAT_Repository\FCSDAT\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2939E5-A3E9-476C-84C5-D803C12E420A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3568D70D-AC3F-4D86-A37F-1EFDF000B329}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19395" windowHeight="10395" xr2:uid="{8965BD36-60C8-4316-B37C-7C2AADE32A35}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{8965BD36-60C8-4316-B37C-7C2AADE32A35}"/>
   </bookViews>
   <sheets>
     <sheet name="FCDATALSU" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>I (A/cm2) 160</t>
   </si>
@@ -57,15 +66,6 @@
   </si>
   <si>
     <t>E_CO(V)220</t>
-  </si>
-  <si>
-    <t>E (V) 160 (Corrected)</t>
-  </si>
-  <si>
-    <t>E (V) 180 (Corrected)</t>
-  </si>
-  <si>
-    <t>Offset =</t>
   </si>
   <si>
     <t>x</t>
@@ -126,15 +126,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -200,7 +197,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>FCDATALSU!$R$2:$R$18</c:f>
+              <c:f>FCDATALSU!$L$2:$L$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="17"/>
@@ -260,7 +257,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>FCDATALSU!$S$2:$S$18</c:f>
+              <c:f>FCDATALSU!$M$2:$M$18</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="17"/>
@@ -656,7 +653,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>FCDATALSU!$G$2:$G$8</c:f>
+              <c:f>FCDATALSU!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="7"/>
@@ -686,7 +683,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>FCDATALSU!$H$2:$H$8</c:f>
+              <c:f>FCDATALSU!$E$2:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2856,13 +2853,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>331305</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>185531</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>637761</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>71231</xdr:rowOff>
@@ -2893,13 +2890,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>646044</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>11596</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>231913</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>87796</xdr:rowOff>
     </xdr:to>
@@ -3269,490 +3266,376 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A238F7C-029F-46C4-8209-F19FFA5AC309}">
-  <dimension ref="A1:S42"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.3984375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.73046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.3984375" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="3">
-        <v>0.17599999999999999</v>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="3">
-        <v>0.20499999999999999</v>
+        <v>5</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="S1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="3">
         <v>0</v>
       </c>
       <c r="B2" s="3">
         <v>0.69279999999999997</v>
       </c>
-      <c r="C2" s="3">
-        <f t="shared" ref="C2:C7" si="0">+B2+$F$1</f>
-        <v>0.86880000000000002</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.68215999999999999</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1E-4</v>
+      </c>
       <c r="G2" s="3">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0.68215999999999999</v>
-      </c>
-      <c r="I2" s="3">
-        <f t="shared" ref="I2:I8" si="1">+H2+$K$1</f>
-        <v>0.88715999999999995</v>
-      </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3">
+        <v>0.72</v>
+      </c>
+      <c r="H2" s="4">
         <v>1E-4</v>
       </c>
-      <c r="M2" s="3">
-        <v>0.72</v>
-      </c>
-      <c r="N2" s="4">
-        <v>1E-4</v>
-      </c>
-      <c r="O2" s="4">
+      <c r="I2" s="4">
         <v>0.94804999999999995</v>
       </c>
-      <c r="P2" s="4">
+      <c r="J2" s="4">
         <v>1.4485999999999999E-4</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="K2" s="4">
         <v>0.70772999999999997</v>
       </c>
-      <c r="R2" s="6">
+      <c r="L2" s="5">
         <v>4.8179000000000001E-4</v>
       </c>
-      <c r="S2" s="1">
+      <c r="M2" s="1">
         <v>0.82343</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="3">
         <v>9.7000000000000003E-2</v>
       </c>
       <c r="B3" s="3">
         <v>0.59952000000000005</v>
       </c>
-      <c r="C3" s="3">
-        <f t="shared" si="0"/>
-        <v>0.77551999999999999</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3">
+        <v>0.11251</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.58814</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.3</v>
+      </c>
       <c r="G3" s="3">
-        <v>0.11251</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0.58814</v>
-      </c>
-      <c r="I3" s="3">
-        <f t="shared" si="1"/>
-        <v>0.79313999999999996</v>
-      </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="M3" s="3">
         <v>0.64659999999999995</v>
       </c>
-      <c r="N3" s="4">
+      <c r="H3" s="4">
         <v>1E-4</v>
       </c>
-      <c r="O3" s="4">
+      <c r="I3" s="4">
         <v>0.94804999999999995</v>
       </c>
-      <c r="P3" s="4">
+      <c r="J3" s="4">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="K3" s="4">
         <v>0.68579999999999997</v>
       </c>
-      <c r="R3" s="6">
+      <c r="L3" s="5">
         <v>2.4079999999999997E-2</v>
       </c>
-      <c r="S3" s="1">
+      <c r="M3" s="1">
         <v>0.78391</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
         <v>0.26200000000000001</v>
       </c>
       <c r="B4" s="3">
         <v>0.50409000000000004</v>
       </c>
-      <c r="C4" s="3">
-        <f t="shared" si="0"/>
-        <v>0.68009000000000008</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.49285000000000001</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.66</v>
+      </c>
       <c r="G4" s="3">
-        <v>0.28499999999999998</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0.49285000000000001</v>
-      </c>
-      <c r="I4" s="3">
-        <f t="shared" si="1"/>
-        <v>0.69784999999999997</v>
-      </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3">
-        <v>0.66</v>
-      </c>
-      <c r="M4" s="3">
         <v>0.55452000000000001</v>
       </c>
-      <c r="N4" s="4">
+      <c r="H4" s="4">
         <v>4.8179000000000001E-4</v>
       </c>
-      <c r="O4" s="4">
+      <c r="I4" s="4">
         <v>0.82343</v>
       </c>
-      <c r="P4" s="4">
+      <c r="J4" s="4">
         <v>0.1</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="K4" s="4">
         <v>0.65400000000000003</v>
       </c>
-      <c r="R4" s="6">
+      <c r="L4" s="5">
         <v>6.0817999999999997E-2</v>
       </c>
-      <c r="S4" s="1">
+      <c r="M4" s="1">
         <v>0.74256999999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="3">
         <v>0.47399999999999998</v>
       </c>
       <c r="B5" s="3">
         <v>0.41026000000000001</v>
       </c>
-      <c r="C5" s="3">
-        <f t="shared" si="0"/>
-        <v>0.58626</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.39767999999999998</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="G5" s="3">
-        <v>0.49399999999999999</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0.39767999999999998</v>
-      </c>
-      <c r="I5" s="3">
-        <f t="shared" si="1"/>
-        <v>0.60267999999999999</v>
-      </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="M5" s="3">
         <v>0.4642</v>
       </c>
-      <c r="N5" s="4">
+      <c r="H5" s="4">
         <v>2.4079999999999997E-2</v>
       </c>
-      <c r="O5" s="4">
+      <c r="I5" s="4">
         <v>0.78391</v>
       </c>
-      <c r="P5" s="4">
+      <c r="J5" s="4">
         <v>0.21493999999999999</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="K5" s="4">
         <v>0.61102999999999996</v>
       </c>
-      <c r="R5">
+      <c r="L5">
         <v>0.12553</v>
       </c>
-      <c r="S5" s="1">
+      <c r="M5" s="1">
         <v>0.70284000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="3">
         <v>0.70399999999999996</v>
       </c>
       <c r="B6" s="3">
         <v>0.31529000000000001</v>
       </c>
-      <c r="C6" s="3">
-        <f t="shared" si="0"/>
-        <v>0.49129</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.30293999999999999</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1.45</v>
+      </c>
       <c r="G6" s="3">
-        <v>0.7</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0.30293999999999999</v>
-      </c>
-      <c r="I6" s="3">
-        <f t="shared" si="1"/>
-        <v>0.50793999999999995</v>
-      </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3">
-        <v>1.45</v>
-      </c>
-      <c r="M6" s="3">
         <v>0.37190000000000001</v>
       </c>
-      <c r="N6" s="4">
+      <c r="H6" s="4">
         <v>6.0817999999999997E-2</v>
       </c>
-      <c r="O6" s="4">
+      <c r="I6" s="4">
         <v>0.74256999999999995</v>
       </c>
-      <c r="P6" s="4">
+      <c r="J6" s="4">
         <v>0.38</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="K6" s="4">
         <v>0.56999999999999995</v>
       </c>
-      <c r="R6">
+      <c r="L6">
         <v>0.22696</v>
       </c>
-      <c r="S6" s="1">
+      <c r="M6" s="1">
         <v>0.66315000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="3">
         <v>0.90200000000000002</v>
       </c>
       <c r="B7" s="3">
         <v>0.22006000000000001</v>
       </c>
-      <c r="C7" s="3">
-        <f t="shared" si="0"/>
-        <v>0.39605999999999997</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3">
+        <v>0.878</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.20685999999999999</v>
+      </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="3">
-        <v>0.878</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0.20685999999999999</v>
-      </c>
-      <c r="I7" s="3">
-        <f t="shared" si="1"/>
-        <v>0.41186</v>
-      </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="4">
+      <c r="G7" s="3"/>
+      <c r="H7" s="4">
         <v>0.12553</v>
       </c>
-      <c r="O7" s="4">
+      <c r="I7" s="4">
         <v>0.70284000000000002</v>
       </c>
-      <c r="P7" s="4">
+      <c r="J7" s="4">
         <v>0.58707000000000009</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="K7" s="4">
         <v>0.51054999999999995</v>
       </c>
-      <c r="R7">
+      <c r="L7">
         <v>0.37242000000000003</v>
       </c>
-      <c r="S7" s="1">
+      <c r="M7" s="1">
         <v>0.62266999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="3">
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.14323</v>
+      </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="3">
-        <v>0.96799999999999997</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0.14323</v>
-      </c>
-      <c r="I8" s="3">
-        <f t="shared" si="1"/>
-        <v>0.34822999999999998</v>
-      </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="4">
+      <c r="G8" s="3"/>
+      <c r="H8" s="4">
         <v>0.20019000000000001</v>
       </c>
-      <c r="O8" s="4">
+      <c r="I8" s="4">
         <v>0.71128000000000002</v>
       </c>
-      <c r="P8" s="4">
+      <c r="J8" s="4">
         <v>0.75</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="K8" s="4">
         <v>0.47</v>
       </c>
-      <c r="R8">
+      <c r="L8">
         <v>0.55476000000000003</v>
       </c>
-      <c r="S8" s="1">
+      <c r="M8" s="1">
         <v>0.58308000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="3"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="4">
+      <c r="H9" s="4">
         <v>0.20019000000000001</v>
       </c>
-      <c r="O9" s="4">
+      <c r="I9" s="4">
         <v>0.71128000000000002</v>
       </c>
-      <c r="P9" s="4">
+      <c r="J9" s="4">
         <v>1.0052000000000001</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="K9" s="4">
         <v>0.41086</v>
       </c>
-      <c r="R9">
+      <c r="L9">
         <v>0.76794000000000007</v>
       </c>
-      <c r="S9" s="1">
+      <c r="M9" s="1">
         <v>0.54249999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="D10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="4">
+      <c r="H10" s="4">
         <v>0.22696</v>
       </c>
-      <c r="O10" s="4">
+      <c r="I10" s="4">
         <v>0.66315000000000002</v>
       </c>
-      <c r="P10" s="4">
+      <c r="J10" s="4">
         <v>1.125</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="K10" s="4">
         <v>0.38</v>
       </c>
-      <c r="R10">
+      <c r="L10">
         <v>0.99299999999999999</v>
       </c>
-      <c r="S10" s="1">
+      <c r="M10" s="1">
         <v>0.50282000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -3760,32 +3643,26 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="4">
+      <c r="H11" s="4">
         <v>0.37242000000000003</v>
       </c>
-      <c r="O11" s="4">
+      <c r="I11" s="4">
         <v>0.62266999999999995</v>
       </c>
-      <c r="P11" s="4">
+      <c r="J11" s="4">
         <v>1.2232000000000001</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="K11" s="4">
         <v>0.35742000000000002</v>
       </c>
-      <c r="R11">
+      <c r="L11">
         <v>1.2227999999999999</v>
       </c>
-      <c r="S11" s="1">
+      <c r="M11" s="1">
         <v>0.46289999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -3793,32 +3670,26 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="4">
+      <c r="H12" s="4">
         <v>0.39981</v>
       </c>
-      <c r="O12" s="4">
+      <c r="I12" s="4">
         <v>0.65934999999999999</v>
       </c>
-      <c r="P12" s="4">
+      <c r="J12" s="4">
         <v>1.3232000000000002</v>
       </c>
-      <c r="Q12" s="4">
+      <c r="K12" s="4">
         <v>0.31</v>
       </c>
-      <c r="R12">
+      <c r="L12">
         <v>1.4517</v>
       </c>
-      <c r="S12" s="1">
+      <c r="M12" s="1">
         <v>0.42231000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -3826,290 +3697,284 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="4">
+      <c r="H13" s="4">
         <v>0.39981</v>
       </c>
-      <c r="O13" s="4">
+      <c r="I13" s="4">
         <v>0.65934999999999999</v>
       </c>
-      <c r="P13" s="4">
+      <c r="J13" s="4">
         <v>1.4232</v>
       </c>
-      <c r="Q13" s="4">
+      <c r="K13" s="4">
         <v>0.28000000000000003</v>
       </c>
-      <c r="R13">
+      <c r="L13">
         <v>1.6577</v>
       </c>
-      <c r="S13" s="1">
+      <c r="M13" s="1">
         <v>0.38266</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="N14" s="4">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="H14" s="4">
         <v>0.55476000000000003</v>
       </c>
-      <c r="O14" s="4">
+      <c r="I14" s="4">
         <v>0.58308000000000004</v>
       </c>
-      <c r="R14">
+      <c r="L14">
         <v>1.8355999999999999</v>
       </c>
-      <c r="S14" s="1">
+      <c r="M14" s="1">
         <v>0.34208</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="N15" s="4">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="H15" s="4">
         <v>0.59987999999999997</v>
       </c>
-      <c r="O15" s="4">
+      <c r="I15" s="4">
         <v>0.61721000000000004</v>
       </c>
-      <c r="R15">
+      <c r="L15">
         <v>1.9693000000000001</v>
       </c>
-      <c r="S15" s="1">
+      <c r="M15" s="1">
         <v>0.30232999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="N16" s="4">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="H16" s="4">
         <v>0.59987999999999997</v>
       </c>
-      <c r="O16" s="4">
+      <c r="I16" s="4">
         <v>0.61721000000000004</v>
       </c>
-      <c r="R16">
+      <c r="L16">
         <v>2.0689000000000002</v>
       </c>
-      <c r="S16" s="1">
+      <c r="M16" s="1">
         <v>0.26263999999999998</v>
       </c>
     </row>
-    <row r="17" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N17" s="4">
+    <row r="17" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="H17" s="4">
         <v>0.76794000000000007</v>
       </c>
-      <c r="O17" s="4">
+      <c r="I17" s="4">
         <v>0.54249999999999998</v>
       </c>
-      <c r="R17">
+      <c r="L17">
         <v>2.1583000000000001</v>
       </c>
-      <c r="S17" s="1">
+      <c r="M17" s="1">
         <v>0.22220999999999999</v>
       </c>
     </row>
-    <row r="18" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N18" s="4">
+    <row r="18" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="H18" s="4">
         <v>0.79982000000000009</v>
       </c>
-      <c r="O18" s="4">
+      <c r="I18" s="4">
         <v>0.57530000000000003</v>
       </c>
-      <c r="R18">
+      <c r="L18">
         <v>2.2526999999999999</v>
       </c>
-      <c r="S18" s="1">
+      <c r="M18" s="1">
         <v>0.18267</v>
       </c>
     </row>
-    <row r="19" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N19" s="4">
+    <row r="19" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="H19" s="4">
         <v>0.79982000000000009</v>
       </c>
-      <c r="O19" s="4">
+      <c r="I19" s="4">
         <v>0.57530000000000003</v>
       </c>
     </row>
-    <row r="20" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N20" s="4">
+    <row r="20" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="H20" s="4">
         <v>0.99299999999999999</v>
       </c>
-      <c r="O20" s="4">
+      <c r="I20" s="4">
         <v>0.50282000000000004</v>
       </c>
     </row>
-    <row r="21" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N21" s="4">
+    <row r="21" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="H21" s="4">
         <v>0.99988999999999995</v>
       </c>
-      <c r="O21" s="4">
+      <c r="I21" s="4">
         <v>0.53036000000000005</v>
       </c>
     </row>
-    <row r="22" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N22" s="4">
+    <row r="22" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="H22" s="4">
         <v>0.99988999999999995</v>
       </c>
-      <c r="O22" s="4">
+      <c r="I22" s="4">
         <v>0.53036000000000005</v>
       </c>
     </row>
-    <row r="23" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N23" s="4">
+    <row r="23" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="H23" s="4">
         <v>1.1997</v>
       </c>
-      <c r="O23" s="4">
+      <c r="I23" s="4">
         <v>0.48632999999999998</v>
       </c>
     </row>
-    <row r="24" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N24" s="4">
+    <row r="24" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="H24" s="4">
         <v>1.1997</v>
       </c>
-      <c r="O24" s="4">
+      <c r="I24" s="4">
         <v>0.48632999999999998</v>
       </c>
     </row>
-    <row r="25" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N25" s="4">
+    <row r="25" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="H25" s="4">
         <v>1.2227999999999999</v>
       </c>
-      <c r="O25" s="4">
+      <c r="I25" s="4">
         <v>0.46289999999999998</v>
       </c>
     </row>
-    <row r="26" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N26" s="4">
+    <row r="26" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="H26" s="4">
         <v>1.3997999999999999</v>
       </c>
-      <c r="O26" s="4">
+      <c r="I26" s="4">
         <v>0.44386999999999999</v>
       </c>
     </row>
-    <row r="27" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N27" s="4">
+    <row r="27" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="H27" s="4">
         <v>1.3997999999999999</v>
       </c>
-      <c r="O27" s="4">
+      <c r="I27" s="4">
         <v>0.44386999999999999</v>
       </c>
     </row>
-    <row r="28" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N28" s="4">
+    <row r="28" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="H28" s="4">
         <v>1.4517</v>
       </c>
-      <c r="O28" s="4">
+      <c r="I28" s="4">
         <v>0.42231000000000002</v>
       </c>
     </row>
-    <row r="29" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N29" s="4">
+    <row r="29" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="H29" s="4">
         <v>1.6</v>
       </c>
-      <c r="O29" s="4">
+      <c r="I29" s="4">
         <v>0.40310000000000001</v>
       </c>
     </row>
-    <row r="30" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N30" s="4">
+    <row r="30" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="H30" s="4">
         <v>1.6</v>
       </c>
-      <c r="O30" s="4">
+      <c r="I30" s="4">
         <v>0.40310000000000001</v>
       </c>
     </row>
-    <row r="31" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N31" s="4">
+    <row r="31" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="H31" s="4">
         <v>1.6577</v>
       </c>
-      <c r="O31" s="4">
+      <c r="I31" s="4">
         <v>0.38266</v>
       </c>
     </row>
-    <row r="32" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N32" s="4">
+    <row r="32" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="H32" s="4">
         <v>1.8</v>
       </c>
-      <c r="O32" s="4">
+      <c r="I32" s="4">
         <v>0.36571999999999999</v>
       </c>
     </row>
-    <row r="33" spans="14:15" x14ac:dyDescent="0.25">
-      <c r="N33" s="4">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H33" s="4">
         <v>1.8</v>
       </c>
-      <c r="O33" s="4">
+      <c r="I33" s="4">
         <v>0.36571999999999999</v>
       </c>
     </row>
-    <row r="34" spans="14:15" x14ac:dyDescent="0.25">
-      <c r="N34" s="4">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H34" s="4">
         <v>1.8355999999999999</v>
       </c>
-      <c r="O34" s="4">
+      <c r="I34" s="4">
         <v>0.34208</v>
       </c>
     </row>
-    <row r="35" spans="14:15" x14ac:dyDescent="0.25">
-      <c r="N35" s="4">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H35" s="4">
         <v>1.9693000000000001</v>
       </c>
-      <c r="O35" s="4">
+      <c r="I35" s="4">
         <v>0.30232999999999999</v>
       </c>
     </row>
-    <row r="36" spans="14:15" x14ac:dyDescent="0.25">
-      <c r="N36" s="4">
+    <row r="36" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H36" s="4">
         <v>2.0004</v>
       </c>
-      <c r="O36" s="4">
+      <c r="I36" s="4">
         <v>0.3286</v>
       </c>
     </row>
-    <row r="37" spans="14:15" x14ac:dyDescent="0.25">
-      <c r="N37" s="4">
+    <row r="37" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H37" s="4">
         <v>2.0004</v>
       </c>
-      <c r="O37" s="4">
+      <c r="I37" s="4">
         <v>0.3286</v>
       </c>
     </row>
-    <row r="38" spans="14:15" x14ac:dyDescent="0.25">
-      <c r="N38" s="4">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H38" s="4">
         <v>2.0689000000000002</v>
       </c>
-      <c r="O38" s="4">
+      <c r="I38" s="4">
         <v>0.26263999999999998</v>
       </c>
     </row>
-    <row r="39" spans="14:15" x14ac:dyDescent="0.25">
-      <c r="N39" s="4">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H39" s="4">
         <v>2.1583000000000001</v>
       </c>
-      <c r="O39" s="4">
+      <c r="I39" s="4">
         <v>0.22220999999999999</v>
       </c>
     </row>
-    <row r="40" spans="14:15" x14ac:dyDescent="0.25">
-      <c r="N40" s="4">
+    <row r="40" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H40" s="4">
         <v>2.2000999999999999</v>
       </c>
-      <c r="O40" s="4">
+      <c r="I40" s="4">
         <v>0.28405000000000002</v>
       </c>
     </row>
-    <row r="41" spans="14:15" x14ac:dyDescent="0.25">
-      <c r="N41" s="4">
+    <row r="41" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H41" s="4">
         <v>2.2000999999999999</v>
       </c>
-      <c r="O41" s="4">
+      <c r="I41" s="4">
         <v>0.28405000000000002</v>
       </c>
     </row>
-    <row r="42" spans="14:15" x14ac:dyDescent="0.25">
-      <c r="N42" s="4">
+    <row r="42" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H42" s="4">
         <v>2.2526999999999999</v>
       </c>
-      <c r="O42" s="4">
+      <c r="I42" s="4">
         <v>0.18267</v>
       </c>
     </row>
@@ -4127,7 +3992,7 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4141,40 +4006,40 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
       <c r="G1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4201,7 +4066,7 @@
         <v>0.71751412429378536</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>30</v>
       </c>
@@ -4228,7 +4093,7 @@
         <v>0.71181556195965423</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>40</v>
       </c>
@@ -4255,7 +4120,7 @@
         <v>0.68847352024922115</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>50</v>
       </c>
@@ -4282,7 +4147,7 @@
         <v>0.72067039106145248</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>60</v>
       </c>
@@ -4309,7 +4174,7 @@
         <v>0.74160206718346255</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>100</v>
       </c>

</xml_diff>